<commit_message>
Clearing Efficiency Preliminary Analysis
</commit_message>
<xml_diff>
--- a/fieldwork/datasheets/ClearingEfficiency.xlsx
+++ b/fieldwork/datasheets/ClearingEfficiency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4f5e485ed766aa2/Pictures/Documents/Journal Publications/Manuscripts/Dissertation/CH2_Pomacea-Time-Series/fieldwork/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{A048BE22-6018-4C4D-9790-5004694CDF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{839DAB52-ADF1-4B0C-B104-61229D867183}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{A048BE22-6018-4C4D-9790-5004694CDF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDF26D5B-22A8-45AD-9282-0ECDA8B24856}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{76BAFC61-03AF-47BC-9146-10A1E4391494}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="83">
   <si>
     <t>Clearing Efficiency of Apple Snails</t>
   </si>
@@ -157,13 +157,142 @@
   </si>
   <si>
     <t>N = no</t>
+  </si>
+  <si>
+    <t>Trial List</t>
+  </si>
+  <si>
+    <t>trial</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>bins</t>
+  </si>
+  <si>
+    <t>G,W</t>
+  </si>
+  <si>
+    <t>G,W,R</t>
+  </si>
+  <si>
+    <t>P,W</t>
+  </si>
+  <si>
+    <t>W,P</t>
+  </si>
+  <si>
+    <t>R,P</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>W,P,R</t>
+  </si>
+  <si>
+    <t>W,R,G</t>
+  </si>
+  <si>
+    <t>R,G</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R,W,G</t>
+  </si>
+  <si>
+    <t>G,R</t>
+  </si>
+  <si>
+    <t>G,P</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>W,P,G</t>
+  </si>
+  <si>
+    <t>P,R,W</t>
+  </si>
+  <si>
+    <t>G,R,W</t>
+  </si>
+  <si>
+    <t>W,R</t>
+  </si>
+  <si>
+    <t>R,G,W</t>
+  </si>
+  <si>
+    <t>W,G</t>
+  </si>
+  <si>
+    <t>G,P,W</t>
+  </si>
+  <si>
+    <t>R,W</t>
+  </si>
+  <si>
+    <t>R,G,P</t>
+  </si>
+  <si>
+    <t>R,W,P</t>
+  </si>
+  <si>
+    <t>W,R,P</t>
+  </si>
+  <si>
+    <t>G,W,P</t>
+  </si>
+  <si>
+    <t>R,P,W</t>
+  </si>
+  <si>
+    <t>P,W,G</t>
+  </si>
+  <si>
+    <t>P,G,W</t>
+  </si>
+  <si>
+    <t>W,G,R</t>
+  </si>
+  <si>
+    <t>G,P,R</t>
+  </si>
+  <si>
+    <t>P,R,G</t>
+  </si>
+  <si>
+    <t>W,G,P</t>
+  </si>
+  <si>
+    <t>Blind</t>
+  </si>
+  <si>
+    <t>Blind:</t>
+  </si>
+  <si>
+    <t>C = Complete</t>
+  </si>
+  <si>
+    <t>S = Semi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,16 +308,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -286,11 +429,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -316,6 +520,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,6 +548,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -630,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212779D0-5EFB-4909-A8D1-1DB9646F6B43}">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,10 +869,11 @@
     <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.88671875" customWidth="1"/>
     <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.88671875" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" customWidth="1"/>
+    <col min="13" max="13" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -666,8 +888,9 @@
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="12"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -680,8 +903,9 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:13" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -712,12 +936,15 @@
       <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="11"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="11"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -728,10 +955,11 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K4" s="3"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -742,12 +970,13 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3"/>
+      <c r="L5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -758,12 +987,13 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3"/>
+      <c r="L6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -774,12 +1004,13 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -790,10 +1021,11 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K8" s="3"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -804,12 +1036,13 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -820,12 +1053,13 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="3"/>
+      <c r="L10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -836,12 +1070,13 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="3"/>
+      <c r="L11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -852,12 +1087,13 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="3"/>
+      <c r="L12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -868,12 +1104,13 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="3"/>
+      <c r="L13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -884,10 +1121,11 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K14" s="3"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -898,12 +1136,13 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="3"/>
+      <c r="L15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -914,12 +1153,13 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3"/>
+      <c r="L16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -930,12 +1170,13 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="3"/>
+      <c r="L17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -946,12 +1187,13 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="3"/>
+      <c r="L18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -962,10 +1204,11 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="8"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K19" s="3"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -976,10 +1219,11 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="8"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K20" s="3"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -990,12 +1234,13 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="8"/>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="3"/>
+      <c r="L21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1006,12 +1251,13 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="8"/>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="3"/>
+      <c r="L22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1022,12 +1268,13 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="8"/>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="3"/>
+      <c r="L23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1038,12 +1285,13 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="8"/>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="3"/>
+      <c r="L24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1054,10 +1302,11 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="8"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="5"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K25" s="3"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1068,12 +1317,13 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="3"/>
+      <c r="L26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L26" s="5"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1084,12 +1334,13 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="3"/>
+      <c r="L27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L27" s="5"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1100,10 +1351,11 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K28" s="3"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1114,12 +1366,13 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="8"/>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="3"/>
+      <c r="L29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L29" s="5"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1130,12 +1383,13 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="3"/>
+      <c r="L30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L30" s="5"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1146,14 +1400,15 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="3"/>
+      <c r="L31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="M31" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1164,14 +1419,15 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="3"/>
+      <c r="L32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1182,12 +1438,13 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="3"/>
+      <c r="L33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L33" s="5"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1198,10 +1455,11 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="5"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K34" s="3"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="5"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1212,12 +1470,13 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="4" t="s">
+      <c r="K35" s="3"/>
+      <c r="L35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L35" s="5"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1228,12 +1487,13 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="4" t="s">
+      <c r="K36" s="3"/>
+      <c r="L36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L36" s="5"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1244,12 +1504,13 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="4" t="s">
+      <c r="K37" s="3"/>
+      <c r="L37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L37" s="5"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1260,10 +1521,11 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="5"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K38" s="3"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1274,10 +1536,13 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="5"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K39" s="3"/>
+      <c r="L39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1288,10 +1553,13 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="5"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K40" s="3"/>
+      <c r="L40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M40" s="5"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1302,10 +1570,13 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="8"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="5"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K41" s="3"/>
+      <c r="L41" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1316,10 +1587,11 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="5"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K42" s="3"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1330,10 +1602,11 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="5"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K43" s="3"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1344,10 +1617,11 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="5"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K44" s="3"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="5"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1358,10 +1632,11 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="5"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K45" s="3"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="5"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1372,10 +1647,11 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="5"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K46" s="3"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="5"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1386,10 +1662,11 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="8"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="5"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K47" s="3"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="5"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1400,10 +1677,11 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="5"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K48" s="3"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="5"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1414,10 +1692,11 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="8"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="5"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K49" s="3"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="5"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1428,10 +1707,11 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="7"/>
-    </row>
-    <row r="51" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K50" s="3"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="7"/>
+    </row>
+    <row r="51" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -1462,12 +1742,15 @@
       <c r="J51" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K51" s="10" t="s">
+      <c r="K51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L51" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L51" s="11"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51" s="11"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1478,10 +1761,11 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="5"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K52" s="3"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="5"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1492,10 +1776,11 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="5"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K53" s="3"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="5"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1506,10 +1791,11 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="5"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K54" s="3"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="5"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1520,10 +1806,11 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="5"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K55" s="3"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="5"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1534,10 +1821,11 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="5"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K56" s="3"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="5"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1548,10 +1836,11 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="5"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K57" s="3"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="5"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1562,10 +1851,11 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="5"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K58" s="3"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="5"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1576,10 +1866,11 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="5"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K59" s="3"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="5"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1590,10 +1881,11 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="5"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K60" s="3"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="5"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1604,10 +1896,11 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="5"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K61" s="3"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="5"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1618,10 +1911,11 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="5"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K62" s="3"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="5"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1632,10 +1926,11 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="5"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K63" s="3"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="5"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1646,10 +1941,11 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="5"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K64" s="3"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="5"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1660,10 +1956,11 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="5"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K65" s="3"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="5"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1674,10 +1971,11 @@
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="5"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K66" s="3"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="5"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1688,10 +1986,11 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="5"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K67" s="3"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="5"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1702,10 +2001,11 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="5"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K68" s="3"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="5"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -1716,10 +2016,11 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="5"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K69" s="3"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="5"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -1730,10 +2031,11 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="5"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K70" s="3"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="5"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1744,10 +2046,11 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="5"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K71" s="3"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="5"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -1758,10 +2061,11 @@
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="5"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K72" s="3"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="5"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1772,10 +2076,11 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="5"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K73" s="3"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="5"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1786,10 +2091,11 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="5"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K74" s="3"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="5"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1800,10 +2106,11 @@
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="5"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K75" s="3"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="5"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1814,10 +2121,11 @@
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="5"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K76" s="3"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="5"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1828,10 +2136,11 @@
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="5"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K77" s="3"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="5"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1842,10 +2151,11 @@
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
-      <c r="K78" s="4"/>
-      <c r="L78" s="5"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K78" s="3"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="5"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -1856,10 +2166,11 @@
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="5"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K79" s="3"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="5"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -1870,10 +2181,11 @@
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
-      <c r="K80" s="4"/>
-      <c r="L80" s="5"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K80" s="3"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="5"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -1884,10 +2196,11 @@
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="5"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K81" s="3"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="5"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -1898,10 +2211,11 @@
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
-      <c r="K82" s="4"/>
-      <c r="L82" s="5"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K82" s="3"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="5"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -1912,10 +2226,11 @@
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
-      <c r="K83" s="4"/>
-      <c r="L83" s="5"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K83" s="3"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="5"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -1926,10 +2241,11 @@
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="5"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K84" s="3"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="5"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -1940,10 +2256,11 @@
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="5"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K85" s="3"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="5"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -1954,10 +2271,11 @@
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="5"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K86" s="3"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="5"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -1968,10 +2286,11 @@
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
-      <c r="K87" s="4"/>
-      <c r="L87" s="5"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K87" s="3"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="5"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -1982,10 +2301,11 @@
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
-      <c r="K88" s="4"/>
-      <c r="L88" s="5"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K88" s="3"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="5"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -1996,10 +2316,11 @@
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
-      <c r="K89" s="4"/>
-      <c r="L89" s="5"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K89" s="3"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="5"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -2010,10 +2331,11 @@
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
-      <c r="K90" s="4"/>
-      <c r="L90" s="5"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K90" s="3"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="5"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -2024,10 +2346,11 @@
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
-      <c r="K91" s="4"/>
-      <c r="L91" s="5"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K91" s="3"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="5"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -2038,10 +2361,11 @@
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
-      <c r="K92" s="4"/>
-      <c r="L92" s="5"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K92" s="3"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="5"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -2052,10 +2376,11 @@
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
-      <c r="K93" s="4"/>
-      <c r="L93" s="5"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K93" s="3"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="5"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -2066,10 +2391,11 @@
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
-      <c r="K94" s="4"/>
-      <c r="L94" s="5"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K94" s="3"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="5"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -2080,10 +2406,11 @@
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
-      <c r="K95" s="4"/>
-      <c r="L95" s="5"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K95" s="3"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="5"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -2094,10 +2421,11 @@
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
-      <c r="K96" s="4"/>
-      <c r="L96" s="5"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K96" s="3"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="5"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -2108,10 +2436,11 @@
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
-      <c r="K97" s="4"/>
-      <c r="L97" s="5"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K97" s="3"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="5"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -2122,10 +2451,11 @@
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
-      <c r="K98" s="4"/>
-      <c r="L98" s="5"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K98" s="3"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="5"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -2137,9 +2467,10 @@
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="4"/>
-      <c r="L99" s="5"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L99" s="4"/>
+      <c r="M99" s="5"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -2151,13 +2482,14 @@
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
       <c r="K100" s="6"/>
-      <c r="L100" s="7"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A1:L2"/>
-    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="A1:M2"/>
+    <mergeCell ref="L51:M51"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2166,12 +2498,1807 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0FEB2B-970E-486C-B66C-0B3EA9BB5AE7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" customWidth="1"/>
+    <col min="10" max="10" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.88671875" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" customWidth="1"/>
+    <col min="16" max="16" width="2.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="3">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="3">
+        <v>91</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="3">
+        <v>136</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="18"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="3">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="3">
+        <v>92</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="3">
+        <v>137</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" s="18"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="3">
+        <v>48</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="3">
+        <v>93</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="3">
+        <v>138</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="18"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="3">
+        <v>49</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="3">
+        <v>94</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="3">
+        <v>139</v>
+      </c>
+      <c r="N6" s="3">
+        <v>3</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="18"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="3">
+        <v>50</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="3">
+        <v>95</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="13"/>
+      <c r="M7" s="3">
+        <v>140</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P7" s="18"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="3">
+        <v>51</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="3">
+        <v>96</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="3">
+        <v>141</v>
+      </c>
+      <c r="N8" s="3">
+        <v>2</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="18"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="3">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="3">
+        <v>97</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="3">
+        <v>142</v>
+      </c>
+      <c r="N9" s="3">
+        <v>3</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="3">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="3">
+        <v>98</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="13"/>
+      <c r="M10" s="3">
+        <v>143</v>
+      </c>
+      <c r="N10" s="3">
+        <v>3</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="3">
+        <v>54</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="3">
+        <v>99</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="13"/>
+      <c r="M11" s="3">
+        <v>144</v>
+      </c>
+      <c r="N11" s="3">
+        <v>2</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" s="18"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="3">
+        <v>55</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="3">
+        <v>100</v>
+      </c>
+      <c r="J12" s="3">
+        <v>3</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="3">
+        <v>145</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" s="18"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="3">
+        <v>56</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="3">
+        <v>101</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="3">
+        <v>146</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13" s="18"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="3">
+        <v>57</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="13"/>
+      <c r="I14" s="3">
+        <v>102</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="M14" s="3">
+        <v>147</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P14" s="18"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="3">
+        <v>58</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="3">
+        <v>103</v>
+      </c>
+      <c r="J15" s="3">
+        <v>3</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="13"/>
+      <c r="M15" s="3">
+        <v>148</v>
+      </c>
+      <c r="N15" s="3">
+        <v>2</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P15" s="18"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="3">
+        <v>59</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="3">
+        <v>104</v>
+      </c>
+      <c r="J16" s="3">
+        <v>3</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="13"/>
+      <c r="M16" s="3">
+        <v>149</v>
+      </c>
+      <c r="N16" s="3">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P16" s="18"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="3">
+        <v>60</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="3">
+        <v>105</v>
+      </c>
+      <c r="J17" s="3">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" s="13"/>
+      <c r="M17" s="3">
+        <v>150</v>
+      </c>
+      <c r="N17" s="3">
+        <v>3</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="P17" s="18"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="3">
+        <v>61</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="3">
+        <v>106</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18" s="13"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="18"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="3">
+        <v>62</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="3">
+        <v>107</v>
+      </c>
+      <c r="J19" s="3">
+        <v>3</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="13"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="18"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="3">
+        <v>63</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="3">
+        <v>108</v>
+      </c>
+      <c r="J20" s="3">
+        <v>3</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L20" s="13"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="18"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="3">
+        <v>64</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="3">
+        <v>109</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" s="13"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="18"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="3">
+        <v>65</v>
+      </c>
+      <c r="F22" s="3">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="3">
+        <v>110</v>
+      </c>
+      <c r="J22" s="3">
+        <v>3</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" s="13"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="18"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="3">
+        <v>66</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="3">
+        <v>111</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L23" s="13"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="18"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="3">
+        <v>67</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="3">
+        <v>112</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L24" s="13"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="18"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="3">
+        <v>68</v>
+      </c>
+      <c r="F25" s="3">
+        <v>3</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="3">
+        <v>113</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25" s="13"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="18"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="3">
+        <v>69</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" s="13"/>
+      <c r="I26" s="3">
+        <v>114</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" s="13"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="18"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="3">
+        <v>70</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="13"/>
+      <c r="I27" s="3">
+        <v>115</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L27" s="13"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="18"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="3">
+        <v>71</v>
+      </c>
+      <c r="F28" s="3">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="13"/>
+      <c r="I28" s="3">
+        <v>116</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L28" s="13"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="18"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3">
+        <v>3</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="3">
+        <v>72</v>
+      </c>
+      <c r="F29" s="3">
+        <v>3</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="13"/>
+      <c r="I29" s="3">
+        <v>117</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L29" s="13"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="18"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="3">
+        <v>73</v>
+      </c>
+      <c r="F30" s="3">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="13"/>
+      <c r="I30" s="3">
+        <v>118</v>
+      </c>
+      <c r="J30" s="3">
+        <v>3</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L30" s="13"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="18"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="3">
+        <v>74</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="3">
+        <v>119</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L31" s="13"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="18"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="3">
+        <v>75</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="3">
+        <v>120</v>
+      </c>
+      <c r="J32" s="3">
+        <v>3</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L32" s="13"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="18"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="3">
+        <v>76</v>
+      </c>
+      <c r="F33" s="3">
+        <v>2</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="13"/>
+      <c r="I33" s="3">
+        <v>121</v>
+      </c>
+      <c r="J33" s="3">
+        <v>3</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L33" s="13"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="18"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="3">
+        <v>77</v>
+      </c>
+      <c r="F34" s="3">
+        <v>3</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H34" s="13"/>
+      <c r="I34" s="3">
+        <v>122</v>
+      </c>
+      <c r="J34" s="3">
+        <v>3</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L34" s="13"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="18"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="3">
+        <v>78</v>
+      </c>
+      <c r="F35" s="3">
+        <v>3</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="13"/>
+      <c r="I35" s="3">
+        <v>123</v>
+      </c>
+      <c r="J35" s="3">
+        <v>2</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L35" s="13"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="18"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="3">
+        <v>79</v>
+      </c>
+      <c r="F36" s="3">
+        <v>3</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="3">
+        <v>124</v>
+      </c>
+      <c r="J36" s="3">
+        <v>1</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L36" s="13"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="18"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3">
+        <v>3</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="3">
+        <v>80</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" s="13"/>
+      <c r="I37" s="3">
+        <v>125</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L37" s="13"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="18"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="3">
+        <v>81</v>
+      </c>
+      <c r="F38" s="3">
+        <v>3</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" s="13"/>
+      <c r="I38" s="3">
+        <v>126</v>
+      </c>
+      <c r="J38" s="3">
+        <v>1</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L38" s="13"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="18"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="13"/>
+      <c r="E39" s="3">
+        <v>82</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" s="13"/>
+      <c r="I39" s="3">
+        <v>127</v>
+      </c>
+      <c r="J39" s="3">
+        <v>3</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L39" s="13"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="18"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3">
+        <v>3</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="3">
+        <v>83</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40" s="13"/>
+      <c r="I40" s="3">
+        <v>128</v>
+      </c>
+      <c r="J40" s="3">
+        <v>3</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L40" s="13"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="18"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="3">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="13"/>
+      <c r="E41" s="3">
+        <v>84</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H41" s="13"/>
+      <c r="I41" s="3">
+        <v>129</v>
+      </c>
+      <c r="J41" s="3">
+        <v>3</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L41" s="13"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="18"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="13"/>
+      <c r="E42" s="3">
+        <v>85</v>
+      </c>
+      <c r="F42" s="3">
+        <v>3</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="13"/>
+      <c r="I42" s="3">
+        <v>130</v>
+      </c>
+      <c r="J42" s="3">
+        <v>1</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L42" s="13"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="18"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>41</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="13"/>
+      <c r="E43" s="3">
+        <v>86</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="13"/>
+      <c r="I43" s="3">
+        <v>131</v>
+      </c>
+      <c r="J43" s="3">
+        <v>3</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L43" s="13"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="18"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="13"/>
+      <c r="E44" s="3">
+        <v>87</v>
+      </c>
+      <c r="F44" s="3">
+        <v>2</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H44" s="13"/>
+      <c r="I44" s="3">
+        <v>132</v>
+      </c>
+      <c r="J44" s="3">
+        <v>3</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L44" s="13"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="18"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3">
+        <v>3</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="E45" s="3">
+        <v>88</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H45" s="13"/>
+      <c r="I45" s="3">
+        <v>133</v>
+      </c>
+      <c r="J45" s="3">
+        <v>1</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L45" s="13"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="18"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="13"/>
+      <c r="E46" s="3">
+        <v>89</v>
+      </c>
+      <c r="F46" s="3">
+        <v>2</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H46" s="13"/>
+      <c r="I46" s="3">
+        <v>134</v>
+      </c>
+      <c r="J46" s="3">
+        <v>2</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L46" s="13"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="18"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>45</v>
+      </c>
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="19"/>
+      <c r="E47" s="3">
+        <v>90</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="19"/>
+      <c r="I47" s="3">
+        <v>135</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L47" s="19"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:P1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>